<commit_message>
validaciones listas, y exception
</commit_message>
<xml_diff>
--- a/reporteEntrada.xlsx
+++ b/reporteEntrada.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -47,16 +47,16 @@
     <t>Valor_Compras_totales</t>
   </si>
   <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>Mon Jun 01 18:19:53 COT 2020</t>
-  </si>
-  <si>
-    <t>primera compra</t>
-  </si>
-  <si>
-    <t>21265261</t>
+    <t>82</t>
+  </si>
+  <si>
+    <t>Fri Jun 05 01:56:51 COT 2020</t>
+  </si>
+  <si>
+    <t>compra</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
   <si>
     <t>Admin</t>
@@ -65,85 +65,154 @@
     <t>Compra</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>azucar lb</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>unidades</t>
+  </si>
+  <si>
+    <t>3000.0</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>bombones</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>2500.0</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>Sat Jun 06 01:57:28 COT 2020</t>
+  </si>
+  <si>
+    <t>devolucion</t>
+  </si>
+  <si>
+    <t>DevolucionEntrada</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>frutiño</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>5000.0</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
-    <t>Cepillo Colgate</t>
-  </si>
-  <si>
-    <t>15.0</t>
+    <t>gelatina</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>1800.0</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>Fri Jun 05 01:57:59 COT 2020</t>
+  </si>
+  <si>
+    <t>prestamo</t>
+  </si>
+  <si>
+    <t>PrestamoEntrada</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>vive 100</t>
   </si>
   <si>
     <t>Unidad</t>
   </si>
   <si>
-    <t>22500.0</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Arroz Diana lb</t>
-  </si>
-  <si>
-    <t>31.0</t>
-  </si>
-  <si>
-    <t>46500.0</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Mon Jun 01 18:20:16 COT 2020</t>
-  </si>
-  <si>
-    <t>cepillos colgate</t>
-  </si>
-  <si>
-    <t>1315126</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>7500.0</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>Mon Jun 01 18:48:22 COT 2020</t>
+    <t>87</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>shampoo 10ml</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>6000.0</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>Fri Jun 05 03:00:38 COT 2020</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1500.0</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>500.0</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>Fri Jun 05 03:02:39 COT 2020</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>helado</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>Fri Jun 05 16:35:16 COT 2020</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>23215</t>
-  </si>
-  <si>
-    <t>12.0</t>
-  </si>
-  <si>
-    <t>18000.0</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Atun Isabel</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>16800.0</t>
+    <t>1000.0</t>
   </si>
 </sst>
 </file>
@@ -313,103 +382,243 @@
         <v>29</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
         <v>42</v>
       </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
         <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="L11" t="n">
-        <v>111300.0</v>
+        <v>24800.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>